<commit_message>
Atualiza planilha com novos dados
</commit_message>
<xml_diff>
--- a/APP do Leão.xlsx
+++ b/APP do Leão.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2910d0e3dffd63c/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Curso - Dio - Excel com IA\App do Leão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1187" documentId="8_{E5994BCE-F765-4A5E-AB4F-06C6E54D0736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6735023-8D7D-4C9E-BA95-F424A5F15EF3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA745DB-D234-4432-8004-731C4CD6B105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="36" xr2:uid="{9761876F-2FB8-4EE8-B61D-5ABCC41D682C}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="551" xr2:uid="{9761876F-2FB8-4EE8-B61D-5ABCC41D682C}"/>
   </bookViews>
   <sheets>
     <sheet name="TÍTULAR" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1296,6 +1296,7 @@
     <xf numFmtId="168" fontId="23" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="17" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
@@ -1308,11 +1309,17 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
@@ -1321,13 +1328,6 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
@@ -2184,6 +2184,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-73BA-45FF-BDAD-5DE89891BF52}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2205,6 +2210,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-73BA-45FF-BDAD-5DE89891BF52}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2226,6 +2236,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-73BA-45FF-BDAD-5DE89891BF52}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2247,6 +2262,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-73BA-45FF-BDAD-5DE89891BF52}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -8538,10 +8558,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -8888,11 +8904,11 @@
     </row>
     <row r="4" spans="1:5" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -9033,7 +9049,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9051,19 +9067,19 @@
     </row>
     <row r="3" spans="1:5" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
     </row>
     <row r="4" spans="1:5" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -9076,11 +9092,11 @@
     </row>
     <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="C7" s="96">
+      <c r="C7" s="97">
         <f>SUM(D11,D16,D21,D26,D31,D36,D41)</f>
         <v>7886</v>
       </c>
-      <c r="D7" s="97"/>
+      <c r="D7" s="98"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -9290,7 +9306,7 @@
       <c r="D42" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C7:D7"/>
@@ -9318,7 +9334,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C9" sqref="C9"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
           <xlsdti:showDataTypeIcons visible="0"/>
@@ -9353,27 +9369,27 @@
     </row>
     <row r="3" spans="1:16" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
     </row>
     <row r="4" spans="1:16" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -9383,24 +9399,24 @@
     </row>
     <row r="7" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
       <c r="J7" s="35"/>
-      <c r="K7" s="98" t="s">
+      <c r="K7" s="100" t="s">
         <v>120</v>
       </c>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="98"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="100"/>
+      <c r="P7" s="100"/>
     </row>
     <row r="8" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -9512,14 +9528,14 @@
       <c r="F10" s="44">
         <v>1543</v>
       </c>
-      <c r="G10" s="103">
+      <c r="G10" s="94">
         <f>IF(F10&lt;=1518,F10*0.075,
  IF(F10&lt;=2793.88,F10*0.09-15.18,
   IF(F10&lt;=4190.83,F10*0.12-78.38,
    IF(F10&lt;=8157.41,F10*0.14-141.05,"Acima do teto"))))</f>
         <v>123.69</v>
       </c>
-      <c r="H10" s="103">
+      <c r="H10" s="94">
         <f>IF(F10&lt;=2112,0,
  IF(F10&lt;=2826.65,F10*0.075-158.4,
   IF(F10&lt;=3751.05,F10*0.15-370.4,
@@ -9527,7 +9543,7 @@
     F10*0.275-884.96))))</f>
         <v>0</v>
       </c>
-      <c r="I10" s="103">
+      <c r="I10" s="94">
         <f>IF(F10 - G10 - H10 &lt; 0, 0, F10 - G10 - H10)</f>
         <v>1419.31</v>
       </c>
@@ -9594,15 +9610,15 @@
       <c r="F12" s="44">
         <v>258</v>
       </c>
-      <c r="G12" s="103">
+      <c r="G12" s="94">
         <f t="shared" si="0"/>
         <v>19.349999999999998</v>
       </c>
-      <c r="H12" s="103">
+      <c r="H12" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="103">
+      <c r="I12" s="94">
         <f t="shared" ref="I12:I39" si="2">IF(F12 - G12 - H12 &lt; 0, 0, F12 - G12 - H12)</f>
         <v>238.65</v>
       </c>
@@ -9658,15 +9674,15 @@
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
       <c r="F14" s="44"/>
-      <c r="G14" s="103">
+      <c r="G14" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="103">
+      <c r="H14" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" s="103">
+      <c r="I14" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9710,11 +9726,11 @@
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="44"/>
-      <c r="G16" s="103">
+      <c r="G16" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="103">
+      <c r="H16" s="94">
         <f>IF(F16&lt;=2112,0,
  IF(F16&lt;=2826.65,F16*0.075-158.4,
   IF(F16&lt;=3751.05,F16*0.15-370.4,
@@ -9722,7 +9738,7 @@
     F16*0.275-884.96))))</f>
         <v>0</v>
       </c>
-      <c r="I16" s="103">
+      <c r="I16" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9766,15 +9782,15 @@
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
       <c r="F18" s="44"/>
-      <c r="G18" s="103">
+      <c r="G18" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="103">
+      <c r="H18" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I18" s="103">
+      <c r="I18" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9818,15 +9834,15 @@
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
       <c r="F20" s="44"/>
-      <c r="G20" s="103">
+      <c r="G20" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="103">
+      <c r="H20" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20" s="103">
+      <c r="I20" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9874,15 +9890,15 @@
       <c r="D22" s="43"/>
       <c r="E22" s="43"/>
       <c r="F22" s="44"/>
-      <c r="G22" s="103">
+      <c r="G22" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="103">
+      <c r="H22" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22" s="103">
+      <c r="I22" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9926,15 +9942,15 @@
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
       <c r="F24" s="44"/>
-      <c r="G24" s="103">
+      <c r="G24" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="103">
+      <c r="H24" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I24" s="103">
+      <c r="I24" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9977,15 +9993,15 @@
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
       <c r="F26" s="44"/>
-      <c r="G26" s="103">
+      <c r="G26" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="103">
+      <c r="H26" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I26" s="103">
+      <c r="I26" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10027,15 +10043,15 @@
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="44"/>
-      <c r="G28" s="103">
+      <c r="G28" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H28" s="103">
+      <c r="H28" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I28" s="103">
+      <c r="I28" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10077,15 +10093,15 @@
       <c r="D30" s="43"/>
       <c r="E30" s="43"/>
       <c r="F30" s="44"/>
-      <c r="G30" s="103">
+      <c r="G30" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H30" s="103">
+      <c r="H30" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I30" s="103">
+      <c r="I30" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10127,15 +10143,15 @@
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
       <c r="F32" s="44"/>
-      <c r="G32" s="103">
+      <c r="G32" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="103">
+      <c r="H32" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I32" s="103">
+      <c r="I32" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10177,15 +10193,15 @@
       <c r="D34" s="43"/>
       <c r="E34" s="43"/>
       <c r="F34" s="44"/>
-      <c r="G34" s="103">
+      <c r="G34" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="103">
+      <c r="H34" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I34" s="103">
+      <c r="I34" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10227,15 +10243,15 @@
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
       <c r="F36" s="44"/>
-      <c r="G36" s="103">
+      <c r="G36" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H36" s="103">
+      <c r="H36" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I36" s="103">
+      <c r="I36" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10280,15 +10296,15 @@
       <c r="D38" s="43"/>
       <c r="E38" s="43"/>
       <c r="F38" s="44"/>
-      <c r="G38" s="103">
+      <c r="G38" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H38" s="103">
+      <c r="H38" s="94">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I38" s="103">
+      <c r="I38" s="94">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10360,7 +10376,7 @@
       <c r="H41" s="48"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="K7:P7"/>
     <mergeCell ref="C3:I3"/>
@@ -10433,19 +10449,19 @@
     </row>
     <row r="3" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
     </row>
     <row r="4" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -11029,20 +11045,20 @@
     </row>
     <row r="3" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -11051,11 +11067,11 @@
     </row>
     <row r="6" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="18" thickTop="1" x14ac:dyDescent="0.3">
@@ -11179,11 +11195,11 @@
     </row>
     <row r="16" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="C16" s="101" t="s">
+      <c r="C16" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -11259,11 +11275,11 @@
       <c r="A25" s="1"/>
     </row>
     <row r="36" spans="3:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="101" t="s">
+      <c r="C36" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="101"/>
-      <c r="E36" s="101"/>
+      <c r="D36" s="104"/>
+      <c r="E36" s="104"/>
     </row>
     <row r="37" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="3:5" ht="17.25" x14ac:dyDescent="0.3">
@@ -11311,11 +11327,11 @@
       <c r="E42" s="22"/>
     </row>
     <row r="54" spans="3:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="101" t="s">
+      <c r="C54" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="D54" s="101"/>
-      <c r="E54" s="101"/>
+      <c r="D54" s="104"/>
+      <c r="E54" s="104"/>
     </row>
     <row r="55" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="3:5" ht="17.25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Atualiza planilha e adiciona imagens ao repositório
</commit_message>
<xml_diff>
--- a/APP do Leão.xlsx
+++ b/APP do Leão.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Curso - Dio - Excel com IA\App do Leão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0875E7B0-116A-4E44-AF13-9F7642CE5CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E1F6EF-93C5-40CA-ADF9-9066E7B96EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="551" xr2:uid="{9761876F-2FB8-4EE8-B61D-5ABCC41D682C}"/>
   </bookViews>
@@ -1016,7 +1016,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1329,6 +1329,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -8878,7 +8881,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11021,7 +11024,7 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35:F36"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11114,7 +11117,7 @@
       <c r="C10" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="27" t="str">
+      <c r="D10" s="106" t="str">
         <f>IF(OR(TÍTULAR!D7=0,TÍTULAR!D7=""),"-",TÍTULAR!D7)</f>
         <v>-</v>
       </c>

</xml_diff>

<commit_message>
Primeiro commit do novo repositório
</commit_message>
<xml_diff>
--- a/APP do Leão.xlsx
+++ b/APP do Leão.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Curso - Dio - Excel com IA\App do Leão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E1F6EF-93C5-40CA-ADF9-9066E7B96EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD845ED9-5DC1-4DED-AE12-656A1EE4F390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="551" xr2:uid="{9761876F-2FB8-4EE8-B61D-5ABCC41D682C}"/>
   </bookViews>
@@ -693,7 +693,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,8 +765,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1008,6 +1014,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1023,10 +1044,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1332,6 +1349,10 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="13" borderId="21" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -8899,19 +8920,19 @@
     </row>
     <row r="3" spans="1:5" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="1:5" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -8928,21 +8949,21 @@
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="106"/>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -8970,28 +8991,28 @@
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -9070,43 +9091,43 @@
     </row>
     <row r="3" spans="1:5" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="1:5" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="C7" s="97">
+      <c r="C7" s="96">
         <f>SUM(D11,D16,D21,D26,D31,D36,D41)</f>
         <v>7886</v>
       </c>
-      <c r="D7" s="98"/>
+      <c r="D7" s="97"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>18</v>
       </c>
     </row>
@@ -9124,7 +9145,7 @@
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <v>1518</v>
       </c>
     </row>
@@ -9140,7 +9161,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -9158,7 +9179,7 @@
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <v>200</v>
       </c>
     </row>
@@ -9174,7 +9195,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9192,7 +9213,7 @@
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="12">
         <v>650</v>
       </c>
     </row>
@@ -9208,7 +9229,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -9225,7 +9246,7 @@
       <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="12">
         <v>1518</v>
       </c>
     </row>
@@ -9236,7 +9257,7 @@
       <c r="D27" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
     </row>
@@ -9252,7 +9273,7 @@
       <c r="C31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="12">
         <v>4000</v>
       </c>
     </row>
@@ -9263,7 +9284,7 @@
       <c r="D32" s="3"/>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -9277,7 +9298,7 @@
       <c r="C36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="13"/>
+      <c r="D36" s="12"/>
     </row>
     <row r="37" spans="3:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
@@ -9286,7 +9307,7 @@
       <c r="D37" s="3"/>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -9300,7 +9321,7 @@
       <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="13"/>
+      <c r="D41" s="12"/>
     </row>
     <row r="42" spans="3:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
@@ -9372,27 +9393,27 @@
     </row>
     <row r="3" spans="1:16" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
     </row>
     <row r="4" spans="1:16" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -9402,90 +9423,90 @@
     </row>
     <row r="7" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="100" t="s">
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="99" t="s">
         <v>120</v>
       </c>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="99"/>
+      <c r="N7" s="99"/>
+      <c r="O7" s="99"/>
+      <c r="P7" s="99"/>
     </row>
     <row r="8" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="36" t="s">
+      <c r="J8" s="34"/>
+      <c r="K8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L8" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="38" t="s">
+      <c r="M8" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="N8" s="38" t="s">
+      <c r="N8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="38" t="s">
+      <c r="O8" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="P8" s="38" t="s">
+      <c r="P8" s="37" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="C9" s="39">
+      <c r="C9" s="38">
         <v>45292</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="41">
         <v>1518</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G9" s="48">
         <f>IF(F9&lt;=1518,F9*0.075,
  IF(F9&lt;=2793.88,F9*0.09-15.18,
   IF(F9&lt;=4190.83,F9*0.12-78.38,
    IF(F9&lt;=8157.41,F9*0.14-141.05,"Acima do teto"))))</f>
         <v>113.85</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="48">
         <f>IF(F9&lt;=2112,0,
  IF(F9&lt;=2826.65,F9*0.075-158.4,
   IF(F9&lt;=3751.05,F9*0.15-370.4,
@@ -9493,52 +9514,52 @@
     F9*0.275-884.96))))</f>
         <v>0</v>
       </c>
-      <c r="I9" s="49">
+      <c r="I9" s="48">
         <f>IF(F9 - G9 - H9 &lt; 0, 0, F9 - G9 - H9)</f>
         <v>1404.15</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="39">
+      <c r="J9" s="34"/>
+      <c r="K9" s="38">
         <v>45871</v>
       </c>
-      <c r="L9" s="40" t="s">
+      <c r="L9" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="N9" s="42">
+      <c r="N9" s="41">
         <v>600</v>
       </c>
-      <c r="O9" s="42" t="s">
+      <c r="O9" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="42" t="s">
+      <c r="P9" s="41" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="C10" s="39">
+      <c r="C10" s="38">
         <v>45537</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="43">
         <v>1543</v>
       </c>
-      <c r="G10" s="94">
+      <c r="G10" s="93">
         <f>IF(F10&lt;=1518,F10*0.075,
  IF(F10&lt;=2793.88,F10*0.09-15.18,
   IF(F10&lt;=4190.83,F10*0.12-78.38,
    IF(F10&lt;=8157.41,F10*0.14-141.05,"Acima do teto"))))</f>
         <v>123.69</v>
       </c>
-      <c r="H10" s="94">
+      <c r="H10" s="93">
         <f>IF(F10&lt;=2112,0,
  IF(F10&lt;=2826.65,F10*0.075-158.4,
   IF(F10&lt;=3751.05,F10*0.15-370.4,
@@ -9546,40 +9567,40 @@
     F10*0.275-884.96))))</f>
         <v>0</v>
       </c>
-      <c r="I10" s="94">
+      <c r="I10" s="93">
         <f>IF(F10 - G10 - H10 &lt; 0, 0, F10 - G10 - H10)</f>
         <v>1419.31</v>
       </c>
-      <c r="J10" s="35"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
     </row>
     <row r="11" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="C11" s="39">
+      <c r="C11" s="38">
         <v>45568</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="41">
         <v>4567</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G11" s="48">
         <f t="shared" ref="G11:G39" si="0">IF(F11&lt;=1518,F11*0.075,
  IF(F11&lt;=2793.88,F11*0.09-15.18,
   IF(F11&lt;=4190.83,F11*0.12-78.38,
    IF(F11&lt;=8157.41,F11*0.14-141.05,"Acima do teto"))))</f>
         <v>498.3300000000001</v>
       </c>
-      <c r="H11" s="49">
+      <c r="H11" s="48">
         <f t="shared" ref="H11:H39" si="1">IF(F11&lt;=2112,0,
  IF(F11&lt;=2826.65,F11*0.075-158.4,
   IF(F11&lt;=3751.05,F11*0.15-370.4,
@@ -9587,71 +9608,71 @@
     F11*0.275-884.96))))</f>
         <v>375.84500000000003</v>
       </c>
-      <c r="I11" s="49">
+      <c r="I11" s="48">
         <f>IF(F11 - G11 - H11 &lt; 0, 0, F11 - G11 - H11)</f>
         <v>3692.8249999999998</v>
       </c>
-      <c r="J11" s="35"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
     </row>
     <row r="12" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="C12" s="39">
+      <c r="C12" s="38">
         <v>45630</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="43">
         <v>258</v>
       </c>
-      <c r="G12" s="94">
+      <c r="G12" s="93">
         <f t="shared" si="0"/>
         <v>19.349999999999998</v>
       </c>
-      <c r="H12" s="94">
+      <c r="H12" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="94">
+      <c r="I12" s="93">
         <f t="shared" ref="I12:I39" si="2">IF(F12 - G12 - H12 &lt; 0, 0, F12 - G12 - H12)</f>
         <v>238.65</v>
       </c>
-      <c r="J12" s="35"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
     </row>
     <row r="13" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="C13" s="39">
+      <c r="C13" s="38">
         <v>45631</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="41">
         <v>1456</v>
       </c>
-      <c r="G13" s="49">
+      <c r="G13" s="48">
         <f t="shared" si="0"/>
         <v>109.2</v>
       </c>
-      <c r="H13" s="49">
+      <c r="H13" s="48">
         <f>IF(F13&lt;=2112,0,
  IF(F13&lt;=2826.65,F13*0.075-158.4,
   IF(F13&lt;=3751.05,F13*0.15-370.4,
@@ -9659,81 +9680,81 @@
     F13*0.275-884.96))))</f>
         <v>0</v>
       </c>
-      <c r="I13" s="49">
+      <c r="I13" s="48">
         <f t="shared" si="2"/>
         <v>1346.8</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
     </row>
     <row r="14" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="94">
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="94">
+      <c r="H14" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" s="94">
+      <c r="I14" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="35"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
     </row>
     <row r="15" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="49">
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="49">
+      <c r="H15" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15" s="49">
+      <c r="I15" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J15" s="35"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
     </row>
     <row r="16" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="94">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="94">
+      <c r="H16" s="93">
         <f>IF(F16&lt;=2112,0,
  IF(F16&lt;=2826.65,F16*0.075-158.4,
   IF(F16&lt;=3751.05,F16*0.15-370.4,
@@ -9741,133 +9762,133 @@
     F16*0.275-884.96))))</f>
         <v>0</v>
       </c>
-      <c r="I16" s="94">
+      <c r="I16" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="35"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44"/>
     </row>
     <row r="17" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="49">
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="49">
+      <c r="H17" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="49">
+      <c r="I17" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J17" s="35"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
     </row>
     <row r="18" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="94">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="94">
+      <c r="H18" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I18" s="94">
+      <c r="I18" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J18" s="35"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
     </row>
     <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="49">
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="49">
+      <c r="H19" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I19" s="49">
+      <c r="I19" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J19" s="35"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
     </row>
     <row r="20" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="94">
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="94">
+      <c r="H20" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20" s="94">
+      <c r="I20" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J20" s="35"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
     </row>
     <row r="21" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="49">
+      <c r="C21" s="38"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="49">
+      <c r="H21" s="48">
         <f>IF(F21&lt;=2112,0,
  IF(F21&lt;=2826.65,F21*0.075-158.4,
   IF(F21&lt;=3751.05,F21*0.15-370.4,
@@ -9875,508 +9896,508 @@
     F21*0.275-884.96))))</f>
         <v>0</v>
       </c>
-      <c r="I21" s="49">
+      <c r="I21" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J21" s="35"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
     </row>
     <row r="22" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="94">
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="94">
+      <c r="H22" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22" s="94">
+      <c r="I22" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="35"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
     </row>
     <row r="23" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="49">
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" s="49">
+      <c r="H23" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I23" s="49">
+      <c r="I23" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="35"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
     </row>
     <row r="24" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="94">
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="94">
+      <c r="H24" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I24" s="94">
+      <c r="I24" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J24" s="35"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="45"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
     </row>
     <row r="25" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="49">
+      <c r="C25" s="38"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H25" s="49">
+      <c r="H25" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I25" s="49">
+      <c r="I25" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="35"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
     </row>
     <row r="26" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="94">
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="94">
+      <c r="H26" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I26" s="94">
+      <c r="I26" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J26" s="35"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
     </row>
     <row r="27" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="49">
+      <c r="C27" s="38"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H27" s="49">
+      <c r="H27" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I27" s="49">
+      <c r="I27" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="35"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
     </row>
     <row r="28" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="94">
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H28" s="94">
+      <c r="H28" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I28" s="94">
+      <c r="I28" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28" s="35"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
     </row>
     <row r="29" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C29" s="39"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="49">
+      <c r="C29" s="38"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H29" s="49">
+      <c r="H29" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I29" s="49">
+      <c r="I29" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J29" s="35"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="42"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
     </row>
     <row r="30" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="94">
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H30" s="94">
+      <c r="H30" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I30" s="94">
+      <c r="I30" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J30" s="35"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="44"/>
     </row>
     <row r="31" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C31" s="39"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="49">
+      <c r="C31" s="38"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H31" s="49">
+      <c r="H31" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I31" s="49">
+      <c r="I31" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J31" s="35"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
     </row>
     <row r="32" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="94">
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="94">
+      <c r="H32" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I32" s="94">
+      <c r="I32" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J32" s="35"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
+      <c r="P32" s="44"/>
     </row>
     <row r="33" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C33" s="39"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="49">
+      <c r="C33" s="38"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H33" s="49">
+      <c r="H33" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I33" s="49">
+      <c r="I33" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J33" s="35"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="42"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
     </row>
     <row r="34" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="94">
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="94">
+      <c r="H34" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I34" s="94">
+      <c r="I34" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J34" s="35"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="44"/>
-      <c r="N34" s="45"/>
-      <c r="O34" s="45"/>
-      <c r="P34" s="45"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="44"/>
     </row>
     <row r="35" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C35" s="39"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="49">
+      <c r="C35" s="38"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H35" s="49">
+      <c r="H35" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I35" s="49">
+      <c r="I35" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J35" s="35"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
     </row>
     <row r="36" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="94">
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H36" s="94">
+      <c r="H36" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I36" s="94">
+      <c r="I36" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J36" s="35"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="44"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
+      <c r="P36" s="44"/>
     </row>
     <row r="37" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C37" s="39"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="49">
+      <c r="C37" s="38"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="48">
         <f>IF(F37&lt;=1518,F37*0.075,
  IF(F37&lt;=2793.88,F37*0.09-15.18,
   IF(F37&lt;=4190.83,F37*0.12-78.38,
    IF(F37&lt;=8157.41,F37*0.14-141.05,"Acima do teto"))))</f>
         <v>0</v>
       </c>
-      <c r="H37" s="49">
+      <c r="H37" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I37" s="49">
+      <c r="I37" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J37" s="35"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="42"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
     </row>
     <row r="38" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="94">
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H38" s="94">
+      <c r="H38" s="93">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I38" s="94">
+      <c r="I38" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J38" s="35"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="43"/>
-      <c r="M38" s="44"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="45"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="44"/>
     </row>
     <row r="39" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C39" s="39"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="49">
+      <c r="C39" s="38"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H39" s="49">
+      <c r="H39" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I39" s="49">
+      <c r="I39" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J39" s="35"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="42"/>
-      <c r="N39" s="42"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="42"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
     </row>
     <row r="40" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="62">
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="61">
         <f>SUM(F9:F39)</f>
         <v>9342</v>
       </c>
-      <c r="G40" s="61">
+      <c r="G40" s="60">
         <f>SUM(G9:G39)</f>
         <v>864.42000000000019</v>
       </c>
-      <c r="H40" s="61">
+      <c r="H40" s="60">
         <f>SUM(H9:H39)</f>
         <v>375.84500000000003</v>
       </c>
-      <c r="I40" s="61">
+      <c r="I40" s="60">
         <f>SUM(I9:I39)</f>
         <v>8101.7349999999997</v>
       </c>
-      <c r="J40" s="35"/>
-      <c r="K40" s="58"/>
-      <c r="L40" s="58"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="60">
+      <c r="J40" s="34"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="57"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="59">
         <f>SUM(N9:N39)</f>
         <v>600</v>
       </c>
-      <c r="O40" s="60"/>
-      <c r="P40" s="60"/>
+      <c r="O40" s="59"/>
+      <c r="P40" s="59"/>
     </row>
     <row r="41" spans="3:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="H41" s="48"/>
+      <c r="H41" s="47"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
@@ -10438,7 +10459,7 @@
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -10452,19 +10473,19 @@
     </row>
     <row r="3" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
     </row>
     <row r="4" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -10474,502 +10495,502 @@
     </row>
     <row r="7" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="85" t="s">
+      <c r="F7" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="84" t="s">
+      <c r="G7" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="84" t="s">
+      <c r="H7" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="86" t="s">
+      <c r="I7" s="85" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66" t="str">
+      <c r="C8" s="62"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65" t="str">
         <f>IF(F8="NÃO","⚠ Verificar comprovante",IF(F8="SIM","✔ OK",IF(F8="N/A","-","")))</f>
         <v/>
       </c>
-      <c r="H8" s="67"/>
-      <c r="I8" s="68"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="67"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72" t="str">
+      <c r="C9" s="68"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71" t="str">
         <f t="shared" ref="G9:G44" si="0">IF(F9="NÃO","⚠ Verificar comprovante",IF(F9="SIM","✔ OK",IF(F9="N/A","-","")))</f>
         <v/>
       </c>
-      <c r="H9" s="73"/>
-      <c r="I9" s="74"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="73"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66" t="str">
+      <c r="C10" s="62"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72" t="str">
+      <c r="C11" s="68"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="73"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66" t="str">
+      <c r="C12" s="62"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H12" s="66"/>
-      <c r="I12" s="68"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="67"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="72" t="str">
+      <c r="C13" s="75"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="71" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H13" s="80"/>
-      <c r="I13" s="81"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="80"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66" t="str">
+      <c r="C14" s="62"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75" t="str">
+      <c r="C15" s="68"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H15" s="73"/>
-      <c r="I15" s="74"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="73"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66" t="str">
+      <c r="C16" s="62"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H16" s="67"/>
-      <c r="I16" s="68"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75" t="str">
+      <c r="C17" s="68"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H17" s="75"/>
-      <c r="I17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="73"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66" t="str">
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H18" s="66"/>
-      <c r="I18" s="68"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="67"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82" t="str">
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66" t="str">
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H20" s="67"/>
-      <c r="I20" s="68"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="67"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82" t="str">
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66" t="str">
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H22" s="67"/>
-      <c r="I22" s="68"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="67"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82" t="str">
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66" t="str">
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H24" s="67"/>
-      <c r="I24" s="68"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82" t="str">
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="63"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66" t="str">
+      <c r="C26" s="62"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H26" s="67"/>
-      <c r="I26" s="68"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="67"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="82" t="str">
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H27" s="76"/>
-      <c r="I27" s="76"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="63"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66" t="str">
+      <c r="C28" s="62"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H28" s="67"/>
-      <c r="I28" s="68"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="67"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="82"/>
-      <c r="G29" s="82" t="str">
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="63"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66" t="str">
+      <c r="C30" s="62"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H30" s="67"/>
-      <c r="I30" s="68"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="67"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="82" t="str">
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H31" s="76"/>
-      <c r="I31" s="76"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="75"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="63"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="66" t="str">
+      <c r="C32" s="62"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H32" s="67"/>
-      <c r="I32" s="68"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="67"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="82" t="str">
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H33" s="76"/>
-      <c r="I33" s="76"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="63"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="66"/>
-      <c r="G34" s="66" t="str">
+      <c r="C34" s="62"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H34" s="67"/>
-      <c r="I34" s="68"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="67"/>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82" t="str">
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="75"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C36" s="63"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="66" t="str">
+      <c r="C36" s="62"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H36" s="67"/>
-      <c r="I36" s="68"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="67"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82" t="str">
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="63"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="66"/>
-      <c r="G38" s="66" t="str">
+      <c r="C38" s="62"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H38" s="67"/>
-      <c r="I38" s="68"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="67"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82" t="str">
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="75"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="63"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66" t="str">
+      <c r="C40" s="62"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H40" s="67"/>
-      <c r="I40" s="68"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="67"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="82"/>
-      <c r="G41" s="82" t="str">
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="63"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66" t="str">
+      <c r="C42" s="62"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H42" s="67"/>
-      <c r="I42" s="68"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="67"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82" t="str">
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="81"/>
+      <c r="G43" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="75"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C44" s="63"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66" t="str">
+      <c r="C44" s="62"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H44" s="67"/>
-      <c r="I44" s="68"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="67"/>
     </row>
     <row r="45" spans="3:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C45" s="87"/>
-      <c r="D45" s="88" t="s">
+      <c r="C45" s="86"/>
+      <c r="D45" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="93">
+      <c r="E45" s="92">
         <f>SUM(E8:E44)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="89"/>
-      <c r="G45" s="90"/>
-      <c r="H45" s="91"/>
-      <c r="I45" s="92"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="90"/>
+      <c r="I45" s="91"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
@@ -11048,418 +11069,418 @@
     </row>
     <row r="3" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="16"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="16"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="F5" s="16"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="16"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:9" ht="18" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="25" t="str">
+      <c r="D9" s="24" t="str">
         <f>IF(OR(TÍTULAR!D6=0,TÍTULAR!D6=""),"-",TÍTULAR!D6)</f>
         <v>-</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="19"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="106" t="str">
+      <c r="D10" s="105" t="str">
         <f>IF(OR(TÍTULAR!D7=0,TÍTULAR!D7=""),"-",TÍTULAR!D7)</f>
         <v>-</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="19"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="28" t="str">
+      <c r="D11" s="27" t="str">
         <f>IFERROR(IF(OR(TÍTULAR!D8=0,TÍTULAR!D8=""),"-",TÍTULAR!D8),"")</f>
         <v>-</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="19"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="27" t="str">
+      <c r="D12" s="26" t="str">
         <f>IF(OR(TÍTULAR!D10=0,TÍTULAR!D10=""),"-",TÍTULAR!D10)</f>
         <v>-</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="19"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="25" t="str">
+      <c r="D13" s="24" t="str">
         <f>IF(OR(TÍTULAR!D16=0,TÍTULAR!D16=""),"-",TÍTULAR!D16)</f>
         <v>-</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="30" t="str">
+      <c r="D14" s="29" t="str">
         <f>IF(OR(TÍTULAR!D17=0,TÍTULAR!D17=""),"-",TÍTULAR!D17)</f>
         <v>-</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="19"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="16"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="17"/>
+      <c r="E18" s="16"/>
     </row>
     <row r="19" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="30">
         <f>NOTAS!F40</f>
         <v>9342</v>
       </c>
-      <c r="E19" s="22"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="31">
         <f>NOTAS!N40</f>
         <v>600</v>
       </c>
-      <c r="E20" s="22"/>
+      <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="30">
         <f>D19-D20</f>
         <v>8742</v>
       </c>
-      <c r="E21" s="22"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="51">
+      <c r="D22" s="50">
         <f>IF(D21 &gt; 2000, (D21 - 2000) * 0.15, 0)</f>
         <v>1011.3</v>
       </c>
-      <c r="E22" s="22"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="22"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="22"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
     <row r="36" spans="3:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="104" t="s">
+      <c r="C36" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="104"/>
-      <c r="E36" s="104"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="103"/>
     </row>
     <row r="37" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="3:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="17"/>
+      <c r="E38" s="16"/>
     </row>
     <row r="39" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="25">
+      <c r="D39" s="24">
         <f>COUNTIF(DEDUÇÕES!G8:G44,"✔ OK")</f>
         <v>0</v>
       </c>
-      <c r="E39" s="22"/>
+      <c r="E39" s="21"/>
     </row>
     <row r="40" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="27">
+      <c r="D40" s="26">
         <f>COUNTIF(DEDUÇÕES!G8:G44,"⚠ Verificar")</f>
         <v>0</v>
       </c>
-      <c r="E40" s="22"/>
+      <c r="E40" s="21"/>
     </row>
     <row r="41" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="D41" s="57">
+      <c r="D41" s="56">
         <f>COUNTBLANK(DEDUÇÕES!G8:G44)</f>
         <v>37</v>
       </c>
-      <c r="E41" s="22"/>
+      <c r="E41" s="21"/>
     </row>
     <row r="42" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C42" s="52"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="22"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="21"/>
     </row>
     <row r="54" spans="3:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="104" t="s">
+      <c r="C54" s="103" t="s">
         <v>131</v>
       </c>
-      <c r="D54" s="104"/>
-      <c r="E54" s="104"/>
+      <c r="D54" s="103"/>
+      <c r="E54" s="103"/>
     </row>
     <row r="55" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="3:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E56" s="17"/>
+      <c r="E56" s="16"/>
     </row>
     <row r="57" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C57" s="24" t="s">
+      <c r="C57" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D57" s="31" cm="1">
+      <c r="D57" s="30" cm="1">
         <f t="array" ref="D57">SUMPRODUCT((MONTH(NOTAS!C9:C39)=1)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>1518</v>
       </c>
-      <c r="E57" s="22"/>
+      <c r="E57" s="21"/>
     </row>
     <row r="58" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="D58" s="32" cm="1">
+      <c r="D58" s="31" cm="1">
         <f t="array" ref="D58">SUMPRODUCT((MONTH(NOTAS!C9:C39)=2)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>0</v>
       </c>
-      <c r="E58" s="22"/>
+      <c r="E58" s="21"/>
     </row>
     <row r="59" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C59" s="56" t="s">
+      <c r="C59" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="D59" s="31" cm="1">
+      <c r="D59" s="30" cm="1">
         <f t="array" ref="D59">SUMPRODUCT((MONTH(NOTAS!C9:C39)=31)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>0</v>
       </c>
-      <c r="E59" s="22"/>
+      <c r="E59" s="21"/>
     </row>
     <row r="60" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="D60" s="32" cm="1">
+      <c r="D60" s="31" cm="1">
         <f t="array" ref="D60">SUMPRODUCT((MONTH(NOTAS!C9:C39)=4)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C61" s="56" t="s">
+      <c r="C61" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="D61" s="31" cm="1">
+      <c r="D61" s="30" cm="1">
         <f t="array" ref="D61">SUMPRODUCT((MONTH(NOTAS!C9:C39)=5)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="D62" s="32" cm="1">
+      <c r="D62" s="31" cm="1">
         <f t="array" ref="D62">SUMPRODUCT((MONTH(NOTAS!C9:C39)=6)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C63" s="24" t="s">
+      <c r="C63" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D63" s="31" cm="1">
+      <c r="D63" s="30" cm="1">
         <f t="array" ref="D63">SUMPRODUCT((MONTH(NOTAS!C9:C39)=7)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="3:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C64" s="26" t="s">
+      <c r="C64" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="D64" s="32" cm="1">
+      <c r="D64" s="31" cm="1">
         <f t="array" ref="D64">SUMPRODUCT((MONTH(NOTAS!C9:C39)=8)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="3:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="D65" s="31" cm="1">
+      <c r="D65" s="30" cm="1">
         <f t="array" ref="D65">SUMPRODUCT((MONTH(NOTAS!C9:C39)=9)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>1543</v>
       </c>
     </row>
     <row r="66" spans="3:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="32" cm="1">
+      <c r="D66" s="31" cm="1">
         <f t="array" ref="D66">SUMPRODUCT((MONTH(NOTAS!C9:C39)=10)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>4567</v>
       </c>
     </row>
     <row r="67" spans="3:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C67" s="24" t="s">
+      <c r="C67" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D67" s="31" cm="1">
+      <c r="D67" s="30" cm="1">
         <f t="array" ref="D67">SUMPRODUCT((MONTH(NOTAS!C9:C39)=11)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="3:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C68" s="50" t="s">
+      <c r="C68" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="32" cm="1">
+      <c r="D68" s="31" cm="1">
         <f t="array" ref="D68">SUMPRODUCT((MONTH(NOTAS!C9:C39)=12)*(YEAR(NOTAS!C9:C39)=2024)*(NOTAS!F9:F39))</f>
         <v>1714</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C69" s="52"/>
-      <c r="D69" s="53"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="52"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -11526,257 +11547,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="33" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="33" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="33" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="33" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="33" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="33" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="33" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="33" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="33" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="33" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="33" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="33" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="33" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="33" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="33" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="33" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="33" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="33" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="33" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="33" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="33" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="33" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="33" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="33" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="33" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="33" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="33" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="33" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="33" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="33" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="33" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="33" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="33" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>